<commit_message>
BugFix: log transform applied on zero lambda
</commit_message>
<xml_diff>
--- a/data/output/excel/test_trans_XGB-CV-True_ALL.xlsx
+++ b/data/output/excel/test_trans_XGB-CV-True_ALL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omid\Documents\GitHub\research\deep-soil\data\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omid\Documents\GitHub\research\deep-soil\data\output\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,10 @@
   <sheets>
     <sheet name="test_trans_XGB-CV-True_ALL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'test_trans_XGB-CV-True_ALL'!$A$1:$R$57</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1117,11 +1120,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="480693312"/>
-        <c:axId val="480692136"/>
+        <c:axId val="374360072"/>
+        <c:axId val="374364776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="480693312"/>
+        <c:axId val="374360072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,12 +1181,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480692136"/>
+        <c:crossAx val="374364776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="480692136"/>
+        <c:axId val="374364776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +1243,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480693312"/>
+        <c:crossAx val="374360072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1791,11 +1794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="482425968"/>
-        <c:axId val="482424008"/>
+        <c:axId val="374361248"/>
+        <c:axId val="374365168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="482425968"/>
+        <c:axId val="374361248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,12 +1855,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482424008"/>
+        <c:crossAx val="374365168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="482424008"/>
+        <c:axId val="374365168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1914,7 +1917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482425968"/>
+        <c:crossAx val="374361248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2465,11 +2468,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="482425184"/>
-        <c:axId val="482423224"/>
+        <c:axId val="374365952"/>
+        <c:axId val="374362032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="482425184"/>
+        <c:axId val="374365952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2526,12 +2529,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482423224"/>
+        <c:crossAx val="374362032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="482423224"/>
+        <c:axId val="374362032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,7 +2591,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482425184"/>
+        <c:crossAx val="374365952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2741,8 +2744,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.45674723412737966"/>
-                  <c:y val="-0.19769429862933799"/>
+                  <c:x val="-0.42594768468312716"/>
+                  <c:y val="-0.21034583320763064"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2782,34 +2785,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9.9999999999404593E-2</c:v>
@@ -2959,172 +2962,172 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
                 <c:pt idx="0">
-                  <c:v>0.60755192999999996</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83914714999999995</c:v>
+                  <c:v>8.4745762711864403E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28892624</c:v>
+                  <c:v>5.1724137931034482E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8850401</c:v>
+                  <c:v>9.4827586206896547E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48900749999999998</c:v>
+                  <c:v>8.5470085470085472E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.91897505999999995</c:v>
+                  <c:v>0.10619469026548672</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92170819999999998</c:v>
+                  <c:v>7.0796460176991149E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.61650819999999995</c:v>
+                  <c:v>6.7226890756302518E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80928500000000003</c:v>
+                  <c:v>0.10084033613445378</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.70120572999999997</c:v>
+                  <c:v>8.0357142857142863E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20025165</c:v>
+                  <c:v>0.15882352941116928</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.29528743000000002</c:v>
+                  <c:v>0.2150442477870152</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2837306</c:v>
+                  <c:v>0.1689655172407839</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.35162114999999999</c:v>
+                  <c:v>0.23157894736782564</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.22288347999999999</c:v>
+                  <c:v>0.19565217391244807</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.24646387</c:v>
+                  <c:v>0.16140350877133441</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.31153163</c:v>
+                  <c:v>0.18928571428511887</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25782695</c:v>
+                  <c:v>0.17563025210024491</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.28502715000000001</c:v>
+                  <c:v>0.20909090909031369</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.43439737</c:v>
+                  <c:v>0.14237288135533679</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.21933863000000001</c:v>
+                  <c:v>0.22605042016747182</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.29671550000000002</c:v>
+                  <c:v>0.1689655172407839</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.21962835</c:v>
+                  <c:v>0.20909090909031369</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.23686513000000001</c:v>
+                  <c:v>0.17627118644008255</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.31165186</c:v>
+                  <c:v>0.19821428571369032</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.25499073</c:v>
+                  <c:v>0.16249999999940459</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.19667387</c:v>
+                  <c:v>0.29166666675348674</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.23994303</c:v>
+                  <c:v>0.31504424787443069</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.27760132999999998</c:v>
+                  <c:v>0.26034482767302697</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.25427110000000003</c:v>
+                  <c:v>0.24310344836268216</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.25757530000000001</c:v>
+                  <c:v>0.31111111119793122</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.26602796000000001</c:v>
+                  <c:v>0.29243697487673603</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.27282643000000001</c:v>
+                  <c:v>0.29565217399986354</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.2053681</c:v>
+                  <c:v>0.27692307700989705</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.21283162</c:v>
+                  <c:v>0.2598290599158799</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.36662328</c:v>
+                  <c:v>0.25084745771393874</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.32321425999999998</c:v>
+                  <c:v>0.25128205136887138</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.33388396999999997</c:v>
+                  <c:v>0.33513513522195526</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.35564827999999998</c:v>
+                  <c:v>0.27627118652749805</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.23541443000000001</c:v>
+                  <c:v>0.2608695653042114</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.15191509</c:v>
+                  <c:v>0.27142857151539151</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19420607000000001</c:v>
+                  <c:v>0.32820512829194826</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.15236735000000001</c:v>
+                  <c:v>0.30714285722967721</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.22907205999999999</c:v>
+                  <c:v>0.25882352949858478</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.30826472999999999</c:v>
+                  <c:v>0.29734513283018293</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.50566920000000004</c:v>
+                  <c:v>0.32711864415461667</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.20514294999999999</c:v>
+                  <c:v>0.33043478269551574</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.43953249999999999</c:v>
+                  <c:v>0.26306306314988315</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.3880015</c:v>
+                  <c:v>0.28403361353219825</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.36953851999999998</c:v>
+                  <c:v>0.3000000000868201</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.31865009999999999</c:v>
+                  <c:v>0.32931034491440631</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.34275507999999999</c:v>
+                  <c:v>0.29565217399986354</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.37594947000000001</c:v>
+                  <c:v>0.27894736850787272</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.25259735999999999</c:v>
+                  <c:v>0.27500000008682007</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.42853757999999997</c:v>
+                  <c:v>0.32500000008682006</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.28970542999999999</c:v>
+                  <c:v>0.290909090995911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3139,11 +3142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="484778232"/>
-        <c:axId val="484778624"/>
+        <c:axId val="375366840"/>
+        <c:axId val="375372720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="484778232"/>
+        <c:axId val="375366840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3200,12 +3203,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484778624"/>
+        <c:crossAx val="375372720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="484778624"/>
+        <c:axId val="375372720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3262,7 +3265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="484778232"/>
+        <c:crossAx val="375366840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3308,6 +3311,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -5661,68 +5665,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Oval 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1000125" y="8848725"/>
-          <a:ext cx="990600" cy="485775"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-AU" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -6202,6 +6144,164 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.16833</cdr:x>
+      <cdr:y>0.06641</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.37592</cdr:x>
+      <cdr:y>0.26181</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="Oval 1"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="803275" y="165100"/>
+          <a:ext cx="990625" cy="485769"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="lt1">
+            <a:alpha val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6468,7 +6568,7 @@
   <dimension ref="A1:R57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6582,11 +6682,10 @@
         <v>117.25688</v>
       </c>
       <c r="Q2">
-        <f>EXP(I2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.60755192999999996</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -6642,11 +6741,10 @@
         <v>505.49914999999999</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q57" si="3">EXP(I3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>0.83914714999999995</v>
+        <v>8.4745762711864403E-2</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -6702,11 +6800,10 @@
         <v>588.35569999999996</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0.28892624</v>
+        <v>5.1724137931034482E-2</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -6762,11 +6859,10 @@
         <v>1067.6992</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>0.8850401</v>
+        <v>9.4827586206896547E-2</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -6822,11 +6918,10 @@
         <v>1425.9802</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R6">
-        <v>0.48900749999999998</v>
+        <v>8.5470085470085472E-2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -6882,11 +6977,10 @@
         <v>1208.8295000000001</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>0.91897505999999995</v>
+        <v>0.10619469026548672</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -6942,11 +7036,10 @@
         <v>765.8972</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8">
-        <v>0.92170819999999998</v>
+        <v>7.0796460176991149E-2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -7002,11 +7095,10 @@
         <v>493.16287</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9">
-        <v>0.61650819999999995</v>
+        <v>6.7226890756302518E-2</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -7062,11 +7154,10 @@
         <v>1640.5693000000001</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10">
-        <v>0.80928500000000003</v>
+        <v>0.10084033613445378</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -7122,11 +7213,10 @@
         <v>1638.2438</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>0.70120572999999997</v>
+        <v>8.0357142857142863E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -7182,11 +7272,11 @@
         <v>1722.8867</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="Q3:Q57" si="3">EXP(I12)</f>
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R12">
-        <v>0.20025165</v>
+        <v>0.15882352941116928</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -7246,7 +7336,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R13">
-        <v>0.29528743000000002</v>
+        <v>0.2150442477870152</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -7306,7 +7396,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R14">
-        <v>0.2837306</v>
+        <v>0.1689655172407839</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -7366,7 +7456,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R15">
-        <v>0.35162114999999999</v>
+        <v>0.23157894736782564</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -7426,7 +7516,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R16">
-        <v>0.22288347999999999</v>
+        <v>0.19565217391244807</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -7486,7 +7576,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R17">
-        <v>0.24646387</v>
+        <v>0.16140350877133441</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -7546,7 +7636,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R18">
-        <v>0.31153163</v>
+        <v>0.18928571428511887</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -7606,7 +7696,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R19">
-        <v>0.25782695</v>
+        <v>0.17563025210024491</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -7666,7 +7756,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R20">
-        <v>0.28502715000000001</v>
+        <v>0.20909090909031369</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -7726,7 +7816,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R21">
-        <v>0.43439737</v>
+        <v>0.14237288135533679</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -7786,7 +7876,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R22">
-        <v>0.21933863000000001</v>
+        <v>0.22605042016747182</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -7846,7 +7936,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R23">
-        <v>0.29671550000000002</v>
+        <v>0.1689655172407839</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -7906,7 +7996,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R24">
-        <v>0.21962835</v>
+        <v>0.20909090909031369</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -7966,7 +8056,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R25">
-        <v>0.23686513000000001</v>
+        <v>0.17627118644008255</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -8026,7 +8116,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R26">
-        <v>0.31165186</v>
+        <v>0.19821428571369032</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -8086,7 +8176,7 @@
         <v>9.9999999999404593E-2</v>
       </c>
       <c r="R27">
-        <v>0.25499073</v>
+        <v>0.16249999999940459</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -8146,7 +8236,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R28">
-        <v>0.19667387</v>
+        <v>0.29166666675348674</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -8206,7 +8296,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R29">
-        <v>0.23994303</v>
+        <v>0.31504424787443069</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -8266,7 +8356,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R30">
-        <v>0.27760132999999998</v>
+        <v>0.26034482767302697</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -8326,7 +8416,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R31">
-        <v>0.25427110000000003</v>
+        <v>0.24310344836268216</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -8386,7 +8476,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R32">
-        <v>0.25757530000000001</v>
+        <v>0.31111111119793122</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -8446,7 +8536,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R33">
-        <v>0.26602796000000001</v>
+        <v>0.29243697487673603</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -8506,7 +8596,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R34">
-        <v>0.27282643000000001</v>
+        <v>0.29565217399986354</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -8566,7 +8656,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R35">
-        <v>0.2053681</v>
+        <v>0.27692307700989705</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -8626,7 +8716,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R36">
-        <v>0.21283162</v>
+        <v>0.2598290599158799</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -8686,7 +8776,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R37">
-        <v>0.36662328</v>
+        <v>0.25084745771393874</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -8746,7 +8836,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R38">
-        <v>0.32321425999999998</v>
+        <v>0.25128205136887138</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -8806,7 +8896,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R39">
-        <v>0.33388396999999997</v>
+        <v>0.33513513522195526</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -8866,7 +8956,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R40">
-        <v>0.35564827999999998</v>
+        <v>0.27627118652749805</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -8926,7 +9016,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R41">
-        <v>0.23541443000000001</v>
+        <v>0.2608695653042114</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -8986,7 +9076,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R42">
-        <v>0.15191509</v>
+        <v>0.27142857151539151</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -9046,7 +9136,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R43">
-        <v>0.19420607000000001</v>
+        <v>0.32820512829194826</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -9106,7 +9196,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R44">
-        <v>0.15236735000000001</v>
+        <v>0.30714285722967721</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -9166,7 +9256,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R45">
-        <v>0.22907205999999999</v>
+        <v>0.25882352949858478</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -9226,7 +9316,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R46">
-        <v>0.30826472999999999</v>
+        <v>0.29734513283018293</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -9286,7 +9376,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R47">
-        <v>0.50566920000000004</v>
+        <v>0.32711864415461667</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -9346,7 +9436,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R48">
-        <v>0.20514294999999999</v>
+        <v>0.33043478269551574</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -9406,7 +9496,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R49">
-        <v>0.43953249999999999</v>
+        <v>0.26306306314988315</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -9466,7 +9556,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R50">
-        <v>0.3880015</v>
+        <v>0.28403361353219825</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
@@ -9526,7 +9616,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R51">
-        <v>0.36953851999999998</v>
+        <v>0.3000000000868201</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -9586,7 +9676,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R52">
-        <v>0.31865009999999999</v>
+        <v>0.32931034491440631</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -9646,7 +9736,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R53">
-        <v>0.34275507999999999</v>
+        <v>0.29565217399986354</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -9706,7 +9796,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R54">
-        <v>0.37594947000000001</v>
+        <v>0.27894736850787272</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -9766,7 +9856,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R55">
-        <v>0.25259735999999999</v>
+        <v>0.27500000008682007</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -9826,7 +9916,7 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R56">
-        <v>0.42853757999999997</v>
+        <v>0.32500000008682006</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -9886,10 +9976,11 @@
         <v>0.20000000008682009</v>
       </c>
       <c r="R57">
-        <v>0.28970542999999999</v>
+        <v>0.290909090995911</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R57"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>